<commit_message>
done with listing entity for the data catalog
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6537" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6535" uniqueCount="168">
   <si>
     <t>Business Term</t>
   </si>
@@ -439,6 +439,90 @@
   </si>
   <si>
     <t>im.items</t>
+  </si>
+  <si>
+    <t>shoetype</t>
+  </si>
+  <si>
+    <t>The type of the shoes</t>
+  </si>
+  <si>
+    <t>Sandals or Flip Flops</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>The brand of the shoes</t>
+  </si>
+  <si>
+    <t>UnderArmor</t>
+  </si>
+  <si>
+    <t>The color of the shoes</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>character varying(1)</t>
+  </si>
+  <si>
+    <t>The gender the shoes are designed for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F </t>
+  </si>
+  <si>
+    <t>character varying(4)</t>
+  </si>
+  <si>
+    <t>Size of the shoes</t>
+  </si>
+  <si>
+    <t>Condition of the shoes</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>listingprice</t>
+  </si>
+  <si>
+    <t>numeric(8,2)</t>
+  </si>
+  <si>
+    <t>Price set by the seller</t>
+  </si>
+  <si>
+    <t>listingtype</t>
+  </si>
+  <si>
+    <t>character varying(20)</t>
+  </si>
+  <si>
+    <t>Type of the listing</t>
+  </si>
+  <si>
+    <t>Auction</t>
+  </si>
+  <si>
+    <t>listingcreatedate</t>
+  </si>
+  <si>
+    <t>The date at which the listing is created</t>
+  </si>
+  <si>
+    <t>2020-10-06</t>
+  </si>
+  <si>
+    <t>listingenddate</t>
+  </si>
+  <si>
+    <t>The date at which the listing will end</t>
+  </si>
+  <si>
+    <t>2020-11-17</t>
   </si>
 </sst>
 </file>
@@ -1938,412 +2022,412 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="M26" s="14" t="s">
+      <c r="A26" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M27" s="16" t="s">
+      <c r="A27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M27" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="M28" s="14" t="s">
+      <c r="A28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M28" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M29" s="16" t="s">
+      <c r="A29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M29" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="M30" s="14" t="s">
+      <c r="A30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="12">
+        <v>12</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M30" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M31" s="16" t="s">
+      <c r="A31" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L32" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="M32" s="14" t="s">
+      <c r="A32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I32" s="12">
+        <v>52</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M33" s="16" t="s">
+      <c r="A33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M33" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L34" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="M34" s="14" t="s">
+      <c r="A34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M35" s="16" t="s">
+      <c r="A35" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M35" s="13" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
done with the monitoring dashboard
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="257">
   <si>
     <t>Business Term</t>
   </si>
@@ -89,79 +89,58 @@
     <t>Y</t>
   </si>
   <si>
-    <t>BuildingID</t>
-  </si>
-  <si>
-    <t>Apartments</t>
+    <t>Emal</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>False Data</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Some records have fake emails registered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natalie.vitiello@fakeemail.com </t>
+  </si>
+  <si>
+    <t>Users should not register with fake emails</t>
+  </si>
+  <si>
+    <t>All email domain should be checked for validity</t>
+  </si>
+  <si>
+    <t>Number of fake emails ( emails with invalid domains )</t>
+  </si>
+  <si>
+    <t>Totalamount</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>Bad Data</t>
+  </si>
+  <si>
+    <t>Validity</t>
+  </si>
+  <si>
+    <t>Some records have total amount set to zero</t>
+  </si>
+  <si>
+    <t>Total amount of an order should not be zero</t>
+  </si>
+  <si>
+    <t>Number of emails with invalid domains</t>
+  </si>
+  <si>
+    <t>shippingaddress</t>
   </si>
   <si>
     <t>Missing Data</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Some records have NULL values for the BuildingID</t>
-  </si>
-  <si>
-    <t>ApartmentID = 233</t>
-  </si>
-  <si>
-    <t>This field needs to be set to NOT NULL to avoid missing data. &amp;#xA;</t>
-  </si>
-  <si>
-    <t>All apartments must be associated with a building.</t>
-  </si>
-  <si>
-    <t>Number of orphan apartment records (i.e. apartments that are not linked to a building)</t>
-  </si>
-  <si>
-    <t>Emal</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
-    <t>False Data</t>
-  </si>
-  <si>
-    <t>Some records have fake emails registered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natalie.vitiello@fakeemail.com </t>
-  </si>
-  <si>
-    <t>Users should not register with fake emails</t>
-  </si>
-  <si>
-    <t>All email domain should be checked for validity</t>
-  </si>
-  <si>
-    <t>Number of fake emails ( emails with invalid domains )</t>
-  </si>
-  <si>
-    <t>Totalamount</t>
-  </si>
-  <si>
-    <t>Orders</t>
-  </si>
-  <si>
-    <t>Bad Data</t>
-  </si>
-  <si>
-    <t>Validity</t>
-  </si>
-  <si>
-    <t>Some records have total amount set to zero</t>
-  </si>
-  <si>
-    <t>Total amount of an order should not be zero</t>
-  </si>
-  <si>
-    <t>Number of emails with invalid domains</t>
-  </si>
-  <si>
-    <t>shippingaddress</t>
   </si>
   <si>
     <t>Completeness</t>
@@ -1276,60 +1255,60 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1338,7 +1317,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I2" s="8">
         <v>822950</v>
@@ -1347,26 +1326,26 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>22</v>
@@ -1375,339 +1354,339 @@
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I3" s="8">
         <v>3586</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I9" s="8">
         <v>12802</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
@@ -1716,7 +1695,7 @@
         <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I12" s="8">
         <v>2333</v>
@@ -1725,400 +1704,400 @@
         <v>22</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I14" s="8">
         <v>99900</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="I18" s="8">
         <v>14</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>22</v>
@@ -2127,7 +2106,7 @@
         <v>22</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I23" s="8">
         <v>922399</v>
@@ -2136,26 +2115,26 @@
         <v>22</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
       <c r="A24" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>22</v>
@@ -2164,39 +2143,39 @@
         <v>22</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I24" s="8">
         <v>25516</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>22</v>
@@ -2205,418 +2184,418 @@
         <v>22</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I25" s="8">
         <v>509</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
       <c r="A26" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
       <c r="A28" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
       <c r="A29" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
       <c r="A30" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I30" s="8">
         <v>12</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
       <c r="A31" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
       <c r="A32" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I32" s="8">
         <v>52</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
       <c r="A33" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
       <c r="A34" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
       <c r="A35" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
       <c r="A36" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I36" s="8">
         <v>29626</v>
@@ -2628,105 +2607,105 @@
         <v>22</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
       <c r="A37" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I37" s="8">
         <v>998839</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
       <c r="A38" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="I38" s="8">
         <v>45</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="20.25">
       <c r="A39" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>22</v>
@@ -2735,7 +2714,7 @@
         <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I39" s="8">
         <v>29692</v>
@@ -2744,26 +2723,26 @@
         <v>22</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="20.25">
       <c r="A40" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>22</v>
@@ -2772,13 +2751,13 @@
         <v>22</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="I40" s="8">
         <v>7708</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>22</v>
@@ -2788,19 +2767,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="20.25">
       <c r="A41" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>22</v>
@@ -2809,298 +2788,298 @@
         <v>22</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="I41" s="8">
         <v>79220</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
       <c r="A42" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="I42" s="8">
         <v>15.8</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
       <c r="A43" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="I43" s="8">
         <v>9</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
       <c r="A44" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I44" s="8">
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
       <c r="A47" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
       <c r="A48" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
       <c r="A49" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>22</v>
@@ -3109,7 +3088,7 @@
         <v>22</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="I49" s="8">
         <v>797095</v>
@@ -3118,26 +3097,26 @@
         <v>22</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
       <c r="A50" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>22</v>
@@ -3146,150 +3125,150 @@
         <v>22</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I50" s="8">
         <v>427</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
       <c r="A51" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25">
       <c r="A52" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
       <c r="A53" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
       <c r="A54" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>22</v>
@@ -3298,7 +3277,7 @@
         <v>22</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="I54" s="8">
         <v>9467</v>
@@ -3307,100 +3286,100 @@
         <v>22</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
       <c r="A55" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I55" s="8">
         <v>99658816711200</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
       <c r="A56" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
       <c r="A57" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>22</v>
@@ -3409,39 +3388,39 @@
         <v>22</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I57" s="8">
         <v>96342</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
       <c r="A58" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>22</v>
@@ -3450,7 +3429,7 @@
         <v>22</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I58" s="8">
         <v>80527</v>
@@ -3459,192 +3438,192 @@
         <v>22</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
       <c r="A59" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="I63" s="8">
         <v>13835</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -10173,179 +10152,179 @@
         <v>10</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -14286,7 +14265,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -14336,7 +14315,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -14382,22 +14361,22 @@
         <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -14405,124 +14384,92 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="8">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="4"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed the tasks required for phase 1 of this project
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Data Dictionary"/>
@@ -1234,7 +1234,7 @@
   </sheetPr>
   <dimension ref="A1:M496"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14267,7 +14267,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
updated the schema and enterprise conceptual diagram
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="263">
   <si>
     <t>Business Term</t>
   </si>
@@ -266,6 +266,9 @@
     <t>Customer Service System</t>
   </si>
   <si>
+    <t>cs.customerservicerequests</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -278,6 +281,9 @@
     <t>N</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>userid</t>
   </si>
   <si>
@@ -371,6 +377,9 @@
     <t>Inventory Management System</t>
   </si>
   <si>
+    <t>im.items</t>
+  </si>
+  <si>
     <t>itemid</t>
   </si>
   <si>
@@ -488,6 +497,9 @@
     <t>Listing System</t>
   </si>
   <si>
+    <t>li.listings</t>
+  </si>
+  <si>
     <t>listingid</t>
   </si>
   <si>
@@ -503,9 +515,6 @@
     <t>The unique identifier for the product associated to the listing</t>
   </si>
   <si>
-    <t>im.items</t>
-  </si>
-  <si>
     <t>shoetype</t>
   </si>
   <si>
@@ -593,15 +602,18 @@
     <t>Order Processing System</t>
   </si>
   <si>
+    <t>op.orderitems</t>
+  </si>
+  <si>
     <t>The unique ID for each order</t>
   </si>
   <si>
+    <t>op.orderitems.orderid</t>
+  </si>
+  <si>
     <t>The unique ID for the listing that associates to this order</t>
   </si>
   <si>
-    <t>li.listings</t>
-  </si>
-  <si>
     <t>li.listings.listingid</t>
   </si>
   <si>
@@ -695,6 +707,9 @@
     <t>Shipped&amp;#xA;</t>
   </si>
   <si>
+    <t>op.ordershipments</t>
+  </si>
+  <si>
     <t>shipmentid</t>
   </si>
   <si>
@@ -753,6 +768,9 @@
   </si>
   <si>
     <t>Associated user to the credit card</t>
+  </si>
+  <si>
+    <t>usr.users</t>
   </si>
   <si>
     <t>A unique identifier for each user</t>
@@ -1240,7 +1258,7 @@
   <cols>
     <col min="1" max="1" style="5" width="17.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="29.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="26.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="23.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="27.719285714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
@@ -1302,13 +1320,13 @@
         <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1317,7 +1335,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I2" s="8">
         <v>822950</v>
@@ -1326,10 +1344,14 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2" t="s">
@@ -1339,13 +1361,13 @@
         <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>22</v>
@@ -1354,22 +1376,22 @@
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I3" s="8">
         <v>3586</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
@@ -1380,34 +1402,38 @@
         <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2" t="s">
@@ -1417,34 +1443,38 @@
         <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="2" t="s">
@@ -1454,34 +1484,38 @@
         <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="2" t="s">
@@ -1491,34 +1525,38 @@
         <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="2" t="s">
@@ -1528,34 +1566,38 @@
         <v>81</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="2" t="s">
@@ -1565,37 +1607,37 @@
         <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I9" s="8">
         <v>12802</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
@@ -1606,34 +1648,38 @@
         <v>81</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="2" t="s">
@@ -1643,50 +1689,54 @@
         <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
@@ -1695,7 +1745,7 @@
         <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I12" s="8">
         <v>2333</v>
@@ -1704,400 +1754,440 @@
         <v>22</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="I14" s="8">
         <v>99900</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I18" s="8">
         <v>14</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>22</v>
@@ -2106,7 +2196,7 @@
         <v>22</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I23" s="8">
         <v>922399</v>
@@ -2115,26 +2205,30 @@
         <v>22</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
       <c r="A24" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>22</v>
@@ -2143,39 +2237,39 @@
         <v>22</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I24" s="8">
         <v>25516</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>22</v>
@@ -2184,418 +2278,458 @@
         <v>22</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I25" s="8">
         <v>509</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
       <c r="A26" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
       <c r="A28" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
       <c r="A30" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I30" s="8">
         <v>12</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
       <c r="A31" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
       <c r="A32" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I32" s="8">
         <v>52</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
       <c r="A33" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
       <c r="A34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
       <c r="A35" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="F35" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
       <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I36" s="8">
         <v>29626</v>
@@ -2607,10 +2741,10 @@
         <v>22</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>108</v>
+        <v>196</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
@@ -2618,40 +2752,40 @@
         <v>63</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="I37" s="8">
         <v>998839</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
@@ -2659,53 +2793,57 @@
         <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I38" s="8">
         <v>45</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="20.25">
       <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>22</v>
@@ -2714,7 +2852,7 @@
         <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="I39" s="8">
         <v>29692</v>
@@ -2723,26 +2861,30 @@
         <v>22</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="20.25">
       <c r="A40" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>22</v>
@@ -2751,35 +2893,39 @@
         <v>22</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I40" s="8">
         <v>7708</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
+      <c r="L40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="20.25">
       <c r="A41" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>22</v>
@@ -2788,22 +2934,22 @@
         <v>22</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I41" s="8">
         <v>79220</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
@@ -2811,275 +2957,303 @@
         <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="I42" s="8">
         <v>15.8</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
       <c r="A43" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I43" s="8">
         <v>9</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
       <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I44" s="8">
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
       <c r="A45" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
       <c r="A47" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
       <c r="A49" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>22</v>
@@ -3088,7 +3262,7 @@
         <v>22</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="I49" s="8">
         <v>797095</v>
@@ -3097,26 +3271,30 @@
         <v>22</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
       <c r="A50" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>22</v>
@@ -3125,22 +3303,22 @@
         <v>22</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="I50" s="8">
         <v>427</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
@@ -3148,127 +3326,139 @@
         <v>63</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>22</v>
@@ -3277,7 +3467,7 @@
         <v>22</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="I54" s="8">
         <v>9467</v>
@@ -3286,100 +3476,112 @@
         <v>22</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
       <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="I55" s="8">
         <v>99658816711200</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
       <c r="A56" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
       <c r="A57" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>22</v>
@@ -3388,22 +3590,22 @@
         <v>22</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="I57" s="8">
         <v>96342</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M57" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
@@ -3411,16 +3613,16 @@
         <v>67</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>68</v>
+        <v>250</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>22</v>
@@ -3429,7 +3631,7 @@
         <v>22</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="I58" s="8">
         <v>80527</v>
@@ -3438,195 +3640,219 @@
         <v>22</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>68</v>
+        <v>250</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>68</v>
+        <v>250</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>68</v>
+        <v>250</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>68</v>
+        <v>250</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>68</v>
+        <v>250</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="I63" s="8">
         <v>13835</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
       <c r="A64" s="4"/>

</xml_diff>

<commit_message>
fixed the data quality issues columns
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Data Dictionary"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="258">
   <si>
     <t>Business Term</t>
   </si>
@@ -89,10 +89,10 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Emal</t>
-  </si>
-  <si>
-    <t>Users</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>usr.users</t>
   </si>
   <si>
     <t>False Data</t>
@@ -104,7 +104,7 @@
     <t>Some records have fake emails registered</t>
   </si>
   <si>
-    <t xml:space="preserve">natalie.vitiello@fakeemail.com </t>
+    <t xml:space="preserve">email = natalie.vitiello@fakeemail.com </t>
   </si>
   <si>
     <t>Users should not register with fake emails</t>
@@ -116,10 +116,10 @@
     <t>Number of fake emails ( emails with invalid domains )</t>
   </si>
   <si>
-    <t>Totalamount</t>
-  </si>
-  <si>
-    <t>Orders</t>
+    <t>totalamount</t>
+  </si>
+  <si>
+    <t>op.orders</t>
   </si>
   <si>
     <t>Bad Data</t>
@@ -131,6 +131,9 @@
     <t>Some records have total amount set to zero</t>
   </si>
   <si>
+    <t>totalamount = 0</t>
+  </si>
+  <si>
     <t>Total amount of an order should not be zero</t>
   </si>
   <si>
@@ -197,7 +200,7 @@
     <t>items</t>
   </si>
   <si>
-    <t>Items</t>
+    <t>Inventory</t>
   </si>
   <si>
     <t>listings</t>
@@ -323,9 +326,6 @@
     <t>Return</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Email address of the customer contacted</t>
   </si>
   <si>
@@ -347,9 +347,6 @@
     <t>Order ID related to the customer service request</t>
   </si>
   <si>
-    <t>op.orders</t>
-  </si>
-  <si>
     <t>op.orders.orderid</t>
   </si>
   <si>
@@ -371,9 +368,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>Inventory Management System</t>
   </si>
   <si>
@@ -491,9 +485,6 @@
     <t>2020-09-29</t>
   </si>
   <si>
-    <t>Listing</t>
-  </si>
-  <si>
     <t>Listing System</t>
   </si>
   <si>
@@ -662,9 +653,6 @@
     <t>Rate of the tax in percent</t>
   </si>
   <si>
-    <t>totalamount</t>
-  </si>
-  <si>
     <t xml:space="preserve">numeric(8,2)  </t>
   </si>
   <si>
@@ -768,9 +756,6 @@
   </si>
   <si>
     <t>Associated user to the credit card</t>
-  </si>
-  <si>
-    <t>usr.users</t>
   </si>
   <si>
     <t>A unique identifier for each user</t>
@@ -924,9 +909,6 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -937,6 +919,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -1252,11 +1237,11 @@
   </sheetPr>
   <dimension ref="A1:M496"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="23.719285714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="29.14785714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="26.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="23.433571428571426" customWidth="1" bestFit="1"/>
@@ -1273,43 +1258,43 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>76</v>
+      <c r="I1" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
@@ -1317,16 +1302,16 @@
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1335,22 +1320,22 @@
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="8">
+        <v>86</v>
+      </c>
+      <c r="I2" s="12">
         <v>822950</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
@@ -1358,16 +1343,16 @@
         <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>22</v>
@@ -1376,22 +1361,22 @@
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="8">
+        <v>90</v>
+      </c>
+      <c r="I3" s="12">
         <v>3586</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
@@ -1399,40 +1384,40 @@
         <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="I4" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="J4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
@@ -1440,40 +1425,40 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I5" s="8" t="s">
         <v>97</v>
       </c>
+      <c r="I5" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="J5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
@@ -1481,40 +1466,40 @@
         <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I6" s="8" t="s">
         <v>100</v>
       </c>
+      <c r="I6" s="12" t="s">
+        <v>101</v>
+      </c>
       <c r="J6" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
@@ -1522,40 +1507,40 @@
         <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
@@ -1563,40 +1548,40 @@
         <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="12" t="s">
         <v>106</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
@@ -1604,40 +1589,40 @@
         <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="12">
         <v>12802</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
@@ -1645,40 +1630,40 @@
         <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="J10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
@@ -1686,57 +1671,57 @@
         <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
@@ -1745,449 +1730,449 @@
         <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I12" s="8">
+        <v>119</v>
+      </c>
+      <c r="I12" s="12">
         <v>2333</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I14" s="8">
+        <v>125</v>
+      </c>
+      <c r="I14" s="12">
         <v>99900</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="8">
+        <v>139</v>
+      </c>
+      <c r="I18" s="12">
         <v>14</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>143</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I21" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="J21" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D22" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="I22" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="J22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>22</v>
@@ -2196,39 +2181,39 @@
         <v>22</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I23" s="8">
+        <v>158</v>
+      </c>
+      <c r="I23" s="12">
         <v>922399</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
       <c r="A24" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>22</v>
@@ -2237,39 +2222,39 @@
         <v>22</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I24" s="8">
+        <v>159</v>
+      </c>
+      <c r="I24" s="12">
         <v>25516</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>22</v>
@@ -2278,432 +2263,432 @@
         <v>22</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I25" s="8">
+        <v>161</v>
+      </c>
+      <c r="I25" s="12">
         <v>509</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
       <c r="A26" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
       <c r="A28" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I28" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
       <c r="A29" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>175</v>
-      </c>
       <c r="J29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
       <c r="A30" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I30" s="8">
+        <v>174</v>
+      </c>
+      <c r="I30" s="12">
         <v>12</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
       <c r="A31" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
       <c r="A32" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I32" s="8">
+        <v>179</v>
+      </c>
+      <c r="I32" s="12">
         <v>52</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
       <c r="A33" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
       <c r="A34" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
       <c r="A35" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
@@ -2711,27 +2696,27 @@
         <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="I36" s="8">
+        <v>192</v>
+      </c>
+      <c r="I36" s="12">
         <v>29626</v>
       </c>
       <c r="J36" s="2" t="s">
@@ -2741,10 +2726,10 @@
         <v>22</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
@@ -2752,40 +2737,40 @@
         <v>63</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="I37" s="8">
+        <v>194</v>
+      </c>
+      <c r="I37" s="12">
         <v>998839</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
@@ -2793,57 +2778,57 @@
         <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="I38" s="8">
+        <v>198</v>
+      </c>
+      <c r="I38" s="12">
         <v>45</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="20.25">
       <c r="A39" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>22</v>
@@ -2852,39 +2837,39 @@
         <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="I39" s="8">
+        <v>199</v>
+      </c>
+      <c r="I39" s="12">
         <v>29692</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="20.25">
       <c r="A40" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>22</v>
@@ -2893,39 +2878,39 @@
         <v>22</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="I40" s="8">
+        <v>201</v>
+      </c>
+      <c r="I40" s="12">
         <v>7708</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="20.25">
       <c r="A41" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>22</v>
@@ -2934,326 +2919,326 @@
         <v>22</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="I41" s="8">
+        <v>201</v>
+      </c>
+      <c r="I41" s="12">
         <v>79220</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
       <c r="A42" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="I42" s="8">
+        <v>207</v>
+      </c>
+      <c r="I42" s="12">
         <v>15.8</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
       <c r="A43" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="I43" s="8">
+        <v>210</v>
+      </c>
+      <c r="I43" s="12">
         <v>9</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
       <c r="A44" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>214</v>
+        <v>32</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I44" s="8">
+        <v>212</v>
+      </c>
+      <c r="I44" s="12">
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
       <c r="A45" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>214</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>217</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
       <c r="A47" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>225</v>
+        <v>220</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>221</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
       <c r="A48" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
       <c r="A49" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>22</v>
@@ -3262,39 +3247,39 @@
         <v>22</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="I49" s="8">
+        <v>227</v>
+      </c>
+      <c r="I49" s="12">
         <v>797095</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
       <c r="A50" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>22</v>
@@ -3303,145 +3288,145 @@
         <v>22</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="I50" s="8">
+        <v>228</v>
+      </c>
+      <c r="I50" s="12">
         <v>427</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L50" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M50" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
       <c r="A51" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="E51" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>231</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25">
       <c r="A52" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>239</v>
+        <v>234</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>235</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
       <c r="A53" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="I53" s="8" t="s">
-        <v>242</v>
+        <v>237</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
@@ -3449,16 +3434,16 @@
         <v>67</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>22</v>
@@ -3467,22 +3452,22 @@
         <v>22</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="I54" s="8">
+        <v>240</v>
+      </c>
+      <c r="I54" s="12">
         <v>9467</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
@@ -3490,40 +3475,40 @@
         <v>67</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="I55" s="8">
+        <v>242</v>
+      </c>
+      <c r="I55" s="12">
         <v>99658816711200</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
@@ -3531,40 +3516,40 @@
         <v>67</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="E56" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>244</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
@@ -3572,16 +3557,16 @@
         <v>67</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>22</v>
@@ -3590,39 +3575,39 @@
         <v>22</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="I57" s="8">
+        <v>245</v>
+      </c>
+      <c r="I57" s="12">
         <v>96342</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
       <c r="A58" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>250</v>
+        <v>24</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>22</v>
@@ -3631,227 +3616,227 @@
         <v>22</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I58" s="8">
+        <v>246</v>
+      </c>
+      <c r="I58" s="12">
         <v>80527</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
       <c r="A59" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>250</v>
+        <v>24</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="I59" s="8" t="s">
-        <v>253</v>
+        <v>247</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>248</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>250</v>
+        <v>24</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>250</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>250</v>
+        <v>24</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="I61" s="8" t="s">
-        <v>257</v>
+        <v>251</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>252</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>250</v>
+        <v>24</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="I62" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>255</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>250</v>
+        <v>24</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="I63" s="8">
+        <v>257</v>
+      </c>
+      <c r="I63" s="12">
         <v>13835</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
@@ -10374,183 +10359,183 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>51</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -14493,7 +14478,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14503,9 +14488,9 @@
     <col min="4" max="4" style="5" width="13.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="14.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="47.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="29.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="35.14785714285715" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="5" width="79.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="79.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="79.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="79.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -14592,17 +14577,17 @@
       <c r="F3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="8">
-        <v>0</v>
+      <c r="G3" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -14610,31 +14595,31 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -14658,7 +14643,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -14682,7 +14667,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
suggested a future issue with data
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="264">
   <si>
     <t>Business Term</t>
   </si>
@@ -164,6 +164,33 @@
     <t>Number of records with empty shipping address</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>op.ordershipments</t>
+  </si>
+  <si>
+    <t>op.orderitems</t>
+  </si>
+  <si>
+    <t>Consistency</t>
+  </si>
+  <si>
+    <t>Data for order shipment is stored as a date, while the  order date column in in the table 'op.orders' stores data as a timestamp without time zone. This can be problematic in the future, if one wants to catch up and see how an order shipment failed and in which time the error has happened.</t>
+  </si>
+  <si>
+    <t>date = 2020-11-09</t>
+  </si>
+  <si>
+    <t>Make two columns use the same data format</t>
+  </si>
+  <si>
+    <t>Date for order and order shipment should be the same</t>
+  </si>
+  <si>
+    <t>Number of columns with a different data format</t>
+  </si>
+  <si>
     <t>Data Domain</t>
   </si>
   <si>
@@ -281,9 +308,6 @@
     <t>Identifies the unique request made for customer service</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -593,9 +617,6 @@
     <t>Order Processing System</t>
   </si>
   <si>
-    <t>op.orderitems</t>
-  </si>
-  <si>
     <t>The unique ID for each order</t>
   </si>
   <si>
@@ -693,9 +714,6 @@
   </si>
   <si>
     <t>Shipped&amp;#xA;</t>
-  </si>
-  <si>
-    <t>op.ordershipments</t>
   </si>
   <si>
     <t>shipmentid</t>
@@ -1258,60 +1276,60 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1320,7 +1338,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="I2" s="12">
         <v>822950</v>
@@ -1329,30 +1347,30 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>22</v>
@@ -1361,259 +1379,259 @@
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I3" s="12">
         <v>3586</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="I9" s="12">
         <v>12802</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>22</v>
@@ -1622,106 +1640,106 @@
         <v>33</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
@@ -1730,7 +1748,7 @@
         <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="I12" s="12">
         <v>2333</v>
@@ -1739,440 +1757,440 @@
         <v>22</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="I14" s="12">
         <v>99900</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="I18" s="12">
         <v>14</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>22</v>
@@ -2181,7 +2199,7 @@
         <v>22</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="I23" s="12">
         <v>922399</v>
@@ -2190,30 +2208,30 @@
         <v>22</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>22</v>
@@ -2222,39 +2240,39 @@
         <v>22</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="I24" s="12">
         <v>25516</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>22</v>
@@ -2263,458 +2281,458 @@
         <v>22</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="I25" s="12">
         <v>509</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="I30" s="12">
         <v>12</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="I32" s="12">
         <v>52</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
       <c r="A36" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="I36" s="12">
         <v>29626</v>
@@ -2729,106 +2747,106 @@
         <v>33</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="I37" s="12">
         <v>998839</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
       <c r="A38" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="I38" s="12">
         <v>45</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="20.25">
       <c r="A39" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>22</v>
@@ -2837,7 +2855,7 @@
         <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="I39" s="12">
         <v>29692</v>
@@ -2846,30 +2864,30 @@
         <v>22</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="20.25">
       <c r="A40" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>22</v>
@@ -2878,39 +2896,39 @@
         <v>22</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="I40" s="12">
         <v>7708</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="20.25">
       <c r="A41" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>22</v>
@@ -2919,112 +2937,112 @@
         <v>22</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="I41" s="12">
         <v>79220</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
       <c r="A42" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="I42" s="12">
         <v>15.8</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
       <c r="A43" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="I43" s="12">
         <v>9</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
       <c r="A44" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>33</v>
@@ -3033,39 +3051,39 @@
         <v>32</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="I44" s="12">
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
       <c r="A45" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>33</v>
@@ -3074,171 +3092,171 @@
         <v>40</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
       <c r="A46" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
       <c r="A47" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
       <c r="A48" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
       <c r="A49" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>225</v>
+        <v>49</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>22</v>
@@ -3247,7 +3265,7 @@
         <v>22</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="I49" s="12">
         <v>797095</v>
@@ -3256,30 +3274,30 @@
         <v>22</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
       <c r="A50" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>225</v>
+        <v>49</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>22</v>
@@ -3288,13 +3306,13 @@
         <v>22</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="I50" s="12">
         <v>427</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>22</v>
@@ -3303,147 +3321,147 @@
         <v>33</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>225</v>
+        <v>49</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="20.25">
       <c r="A52" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>225</v>
+        <v>49</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="20.25">
       <c r="A53" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>225</v>
+        <v>49</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="20.25">
       <c r="A54" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>22</v>
@@ -3452,7 +3470,7 @@
         <v>22</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="I54" s="12">
         <v>9467</v>
@@ -3461,112 +3479,112 @@
         <v>22</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="20.25">
       <c r="A55" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="I55" s="12">
         <v>99658816711200</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="20.25">
       <c r="A56" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="20.25">
       <c r="A57" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>22</v>
@@ -3575,39 +3593,39 @@
         <v>22</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="I57" s="12">
         <v>96342</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="20.25">
       <c r="A58" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>22</v>
@@ -3616,7 +3634,7 @@
         <v>22</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="I58" s="12">
         <v>80527</v>
@@ -3625,103 +3643,103 @@
         <v>22</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
       <c r="A59" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="20.25">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="20.25">
       <c r="A61" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>24</v>
@@ -3730,113 +3748,113 @@
         <v>23</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="20.25">
       <c r="A62" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="20.25">
       <c r="A63" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="I63" s="12">
         <v>13835</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="20.25">
@@ -10363,179 +10381,179 @@
         <v>10</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -14483,8 +14501,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="15.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="13.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="14.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="47.71928571428572" customWidth="1" bestFit="1"/>
@@ -14494,7 +14512,7 @@
     <col min="10" max="10" style="5" width="79.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -14526,7 +14544,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -14558,7 +14576,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -14590,7 +14608,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -14622,19 +14640,39 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -14646,7 +14684,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -14658,7 +14696,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -14670,7 +14708,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>

</xml_diff>

<commit_message>
updated the metadata to account for the corret data steward
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Data Dictionary"/>
@@ -131,7 +131,7 @@
     <t>Some records have total amount set to zero</t>
   </si>
   <si>
-    <t>totalamount = 0</t>
+    <t>orderid = 29692</t>
   </si>
   <si>
     <t>Total amount of an order should not be zero</t>
@@ -152,7 +152,7 @@
     <t>Some records have no value for the shipping address</t>
   </si>
   <si>
-    <t>orderid = 29626</t>
+    <t>orderid = 13354</t>
   </si>
   <si>
     <t>Address for an order should not be empty</t>
@@ -179,7 +179,7 @@
     <t>Data for order shipment is stored as a date, while the  order date column in in the table 'op.orders' stores data as a timestamp without time zone. This can be problematic in the future, if one wants to catch up and see how an order shipment failed and in which time the error has happened.</t>
   </si>
   <si>
-    <t>date = 2020-11-09</t>
+    <t>shipmentid = 797095</t>
   </si>
   <si>
     <t>Make two columns use the same data format</t>
@@ -221,7 +221,7 @@
     <t>Internal</t>
   </si>
   <si>
-    <t>John Smith</t>
+    <t>Jessica</t>
   </si>
   <si>
     <t>items</t>
@@ -10364,7 +10364,7 @@
   </sheetPr>
   <dimension ref="A1:F500"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14496,7 +14496,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
updated, solved some data in regards to data quality issues
</commit_message>
<xml_diff>
--- a/Copy of SneakerPark Templates.xlsx
+++ b/Copy of SneakerPark Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Data Dictionary"/>
@@ -10364,7 +10364,7 @@
   </sheetPr>
   <dimension ref="A1:F500"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14496,7 +14496,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>